<commit_message>
Fix a couple things in S60003
</commit_message>
<xml_diff>
--- a/tl/S60003.MES.BIN.xlsx
+++ b/tl/S60003.MES.BIN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E227EA0-B858-4A7A-AE25-E64579DC2E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9A1296-3F41-4436-AAEF-DEFF37F6219F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3015" yWindow="6240" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>With that long hair looking like it belongs to an artificial thing, it's Yayoi-san.</t>
+    <t>With that long hair looking like it belongs to something artificial, it's Yayoi-san.</t>
   </si>
   <si>
     <t>Awkward sentence</t>
@@ -104,7 +104,7 @@
     <t>Yayoi</t>
   </si>
   <si>
-    <t>Fujii-san, I assume?</t>
+    <t>Fujii-san, I presume?</t>
   </si>
   <si>
     <t>Was it, Fujii-san?</t>
@@ -1219,7 +1219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>